<commit_message>
etiquetando e alterando notebook
</commit_message>
<xml_diff>
--- a/interface_etiquetagem_tweets/Joker_etiquetada.xlsx
+++ b/interface_etiquetagem_tweets/Joker_etiquetada.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/beatrizcf/2 Semestre - DP/CDADOS/P1_Cdados_BW/interface_etiquetagem_tweets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B3279A3-496F-A440-A1AD-FDC2CE7502AD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24AE6844-FCDF-8046-A985-6F6EEA47A248}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1645,8 +1645,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B301"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" topLeftCell="A279" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD301"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1827,7 +1827,7 @@
         <v>22</v>
       </c>
       <c r="B22">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
@@ -1843,7 +1843,7 @@
         <v>24</v>
       </c>
       <c r="B24">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
@@ -1851,7 +1851,7 @@
         <v>25</v>
       </c>
       <c r="B25">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
@@ -1859,7 +1859,7 @@
         <v>26</v>
       </c>
       <c r="B26">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
@@ -1867,7 +1867,7 @@
         <v>27</v>
       </c>
       <c r="B27">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
@@ -1883,7 +1883,7 @@
         <v>29</v>
       </c>
       <c r="B29">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
@@ -1931,7 +1931,7 @@
         <v>35</v>
       </c>
       <c r="B35">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
@@ -1939,7 +1939,7 @@
         <v>36</v>
       </c>
       <c r="B36">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
@@ -1947,7 +1947,7 @@
         <v>37</v>
       </c>
       <c r="B37">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
@@ -2011,7 +2011,7 @@
         <v>45</v>
       </c>
       <c r="B45">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
@@ -2027,7 +2027,7 @@
         <v>47</v>
       </c>
       <c r="B47">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
@@ -2035,7 +2035,7 @@
         <v>48</v>
       </c>
       <c r="B48">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
@@ -2059,7 +2059,7 @@
         <v>51</v>
       </c>
       <c r="B51">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
@@ -2091,7 +2091,7 @@
         <v>55</v>
       </c>
       <c r="B55">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
@@ -2099,7 +2099,7 @@
         <v>56</v>
       </c>
       <c r="B56">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
@@ -2107,7 +2107,7 @@
         <v>57</v>
       </c>
       <c r="B57">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
@@ -2123,7 +2123,7 @@
         <v>59</v>
       </c>
       <c r="B59">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">
@@ -2139,7 +2139,7 @@
         <v>61</v>
       </c>
       <c r="B61">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">
@@ -2155,7 +2155,7 @@
         <v>63</v>
       </c>
       <c r="B63">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.2">
@@ -2163,7 +2163,7 @@
         <v>64</v>
       </c>
       <c r="B64">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.2">
@@ -2179,7 +2179,7 @@
         <v>66</v>
       </c>
       <c r="B66">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.2">
@@ -2187,7 +2187,7 @@
         <v>67</v>
       </c>
       <c r="B67">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.2">
@@ -2195,7 +2195,7 @@
         <v>68</v>
       </c>
       <c r="B68">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.2">
@@ -2203,7 +2203,7 @@
         <v>69</v>
       </c>
       <c r="B69">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.2">
@@ -2219,7 +2219,7 @@
         <v>71</v>
       </c>
       <c r="B71">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.2">
@@ -2243,7 +2243,7 @@
         <v>74</v>
       </c>
       <c r="B74">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.2">
@@ -2251,7 +2251,7 @@
         <v>75</v>
       </c>
       <c r="B75">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.2">
@@ -2267,7 +2267,7 @@
         <v>77</v>
       </c>
       <c r="B77">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.2">
@@ -2283,7 +2283,7 @@
         <v>79</v>
       </c>
       <c r="B79">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.2">
@@ -2299,7 +2299,7 @@
         <v>81</v>
       </c>
       <c r="B81">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.2">
@@ -2307,7 +2307,7 @@
         <v>82</v>
       </c>
       <c r="B82">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.2">
@@ -2395,7 +2395,7 @@
         <v>93</v>
       </c>
       <c r="B93">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.2">
@@ -2435,7 +2435,7 @@
         <v>98</v>
       </c>
       <c r="B98">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.2">
@@ -2443,7 +2443,7 @@
         <v>99</v>
       </c>
       <c r="B99">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.2">
@@ -2459,7 +2459,7 @@
         <v>101</v>
       </c>
       <c r="B101">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>